<commit_message>
Added the read of the ADC (PA1 - 12 bits).
Readings sent through UART in a formatted DataPacket.
</commit_message>
<xml_diff>
--- a/Resources/DataPacket/DataPacket.xlsx
+++ b/Resources/DataPacket/DataPacket.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Otavi\Documents\Embed\STM32\Projects\DataPacket\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Otavi\Documents\Embed\STM32\Projects\AdcSendRead\Resources\DataPacket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0122F295-5E93-4866-BFBC-D1A4B277E909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39651A3B-3160-4CD6-B47B-F9ED76212921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Packet" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
   <si>
     <t>Start byte 1</t>
   </si>
@@ -130,73 +130,10 @@
     <t>0x7E</t>
   </si>
   <si>
-    <t>0xAA 0x55 0x40 0x02 0x04 0x65 0xF8</t>
-  </si>
-  <si>
-    <t>0x40</t>
-  </si>
-  <si>
-    <t>0x02</t>
-  </si>
-  <si>
-    <t>0xF8</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>0x04 0x65</t>
-  </si>
-  <si>
-    <t>Set the duty cycle to 25%: [1125] = [0x0465]</t>
-  </si>
-  <si>
-    <t>0xAA 0x55 0x40 0x02 0x08 0xCA 0x40</t>
-  </si>
-  <si>
-    <t>0x08 0xCA</t>
-  </si>
-  <si>
-    <t>Set the duty cycle to 50%: [2250] = [0x08CA]</t>
-  </si>
-  <si>
-    <t>0xAA 0x55 0x40 0x02 0x0D 0x2F 0xB4</t>
-  </si>
-  <si>
-    <t>0x0D 0x2F</t>
-  </si>
-  <si>
-    <t>0xB4</t>
-  </si>
-  <si>
-    <t>Set the duty cycle to 75%: [3375] = [0x0D2F]</t>
-  </si>
-  <si>
-    <t>0xAA 0x55 0x40 0x02 0x11 0x94 0x37</t>
-  </si>
-  <si>
-    <t>0x11 0x94</t>
-  </si>
-  <si>
-    <t>0x37</t>
-  </si>
-  <si>
-    <t>Set the duty cycle to 100%: [4500] = [0x1194]</t>
-  </si>
-  <si>
-    <t>0xAA 0x55 0x40 0x02 0x00 0x00 0x90</t>
-  </si>
-  <si>
-    <t>0x00 0x00</t>
-  </si>
-  <si>
-    <t>0x90</t>
-  </si>
-  <si>
-    <t>Set the duty cycle to 0%: [0] = [0x0000]</t>
-  </si>
-  <si>
-    <t>PWM: 20kHz, Duty cycle: [0% - 100%] =&gt; [0 - 4500] = [0x0000 - 0x1194]</t>
+    <t>Makes the led toggles at each 500 miliseconds</t>
   </si>
 </sst>
 </file>
@@ -355,6 +292,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -384,13 +328,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -674,7 +611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BCE9C78-9A57-42A9-943E-E0786B8B6A0B}">
   <dimension ref="A1:NE1136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -691,14 +628,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -1263,13 +1200,13 @@
       <c r="AG6" s="3"/>
     </row>
     <row r="7" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -1300,11 +1237,11 @@
       <c r="AG7" s="3"/>
     </row>
     <row r="8" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="13"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -1335,11 +1272,11 @@
       <c r="AG8" s="3"/>
     </row>
     <row r="9" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="13"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -1370,11 +1307,11 @@
       <c r="AG9" s="3"/>
     </row>
     <row r="10" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="10"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -1405,11 +1342,11 @@
       <c r="AG10" s="3"/>
     </row>
     <row r="11" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="10"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="13"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -1440,11 +1377,11 @@
       <c r="AG11" s="3"/>
     </row>
     <row r="12" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="10"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="13"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -1475,11 +1412,11 @@
       <c r="AG12" s="3"/>
     </row>
     <row r="13" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="10"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="13"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -1510,11 +1447,11 @@
       <c r="AG13" s="3"/>
     </row>
     <row r="14" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="10"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="13"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -1545,11 +1482,11 @@
       <c r="AG14" s="3"/>
     </row>
     <row r="15" spans="1:369" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="10"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="13"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -1580,11 +1517,11 @@
       <c r="AG15" s="3"/>
     </row>
     <row r="16" spans="1:369" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="11"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="13"/>
+      <c r="A16" s="14"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="16"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -40827,10 +40764,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B11DB8B0-5B17-4A82-8032-D4706BCA4450}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40846,11 +40783,11 @@
     <col min="10" max="10" width="62.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -40871,267 +40808,107 @@
       <c r="H1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="16" t="s">
-        <v>33</v>
+      <c r="J1" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="17">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="17">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
-        <v>4</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="17" t="s">
+      <c r="I4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="I5" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="J5" s="17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
-        <v>5</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
-        <v>6</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="J7" s="17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
-        <v>7</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="J8" s="17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="17">
-        <v>8</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="J9" s="17" t="s">
-        <v>51</v>
+      <c r="J4" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a command to enable/disable the sent of ADC readings through serial communication.
</commit_message>
<xml_diff>
--- a/Resources/DataPacket/DataPacket.xlsx
+++ b/Resources/DataPacket/DataPacket.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Otavi\Documents\Embed\STM32\Projects\AdcSendRead\Resources\DataPacket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39651A3B-3160-4CD6-B47B-F9ED76212921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF47FC8-F859-4482-A196-8F211BA0C628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="39">
   <si>
     <t>Start byte 1</t>
   </si>
@@ -134,6 +134,30 @@
   </si>
   <si>
     <t>Makes the led toggles at each 500 miliseconds</t>
+  </si>
+  <si>
+    <t>0x40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xAA 0x55 0x40 0x01 0x00 0x0F </t>
+  </si>
+  <si>
+    <t>0x01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xAA 0x55 0x40 0x01 0x01 0x08 </t>
+  </si>
+  <si>
+    <t>0x08</t>
+  </si>
+  <si>
+    <t>0x0F</t>
+  </si>
+  <si>
+    <t>Disable ADC send read.</t>
+  </si>
+  <si>
+    <t>Enable ADC send read.</t>
   </si>
 </sst>
 </file>
@@ -40764,10 +40788,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B11DB8B0-5B17-4A82-8032-D4706BCA4450}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40911,6 +40935,70 @@
         <v>23</v>
       </c>
     </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>